<commit_message>
ACC_CREATE_ORG - add check quantity before execute loop add data to ACCOUNT, ORGANIZATION sheet add error translate to DefaultValue
</commit_message>
<xml_diff>
--- a/VACCINATION_MANAGEMENT/out/production/VACCINATION_MANAGEMENT/SQL/Data/ACCOUNT.xlsx
+++ b/VACCINATION_MANAGEMENT/out/production/VACCINATION_MANAGEMENT/SQL/Data/ACCOUNT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Project Submission\IS201.M21_20520418_20521252_20521720_20521890\Huong dan cai dat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Projects\VACCINATION\VACCINATION_MANAGEMENT\src\SQL\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
   <si>
     <t>USERNAME</t>
   </si>
@@ -59,13 +59,19 @@
     <t>123</t>
   </si>
   <si>
-    <t>0332743067</t>
-  </si>
-  <si>
-    <t>0332743068</t>
-  </si>
-  <si>
-    <t>0332743069</t>
+    <t>02001</t>
+  </si>
+  <si>
+    <t>02002</t>
+  </si>
+  <si>
+    <t>02003</t>
+  </si>
+  <si>
+    <t>02004</t>
+  </si>
+  <si>
+    <t>02005</t>
   </si>
 </sst>
 </file>
@@ -388,7 +394,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:D8"/>
+      <selection activeCell="D6" sqref="D6:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,11 +480,11 @@
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2">
-        <v>124</v>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -489,10 +495,10 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -502,18 +508,43 @@
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2">
-        <v>125</v>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>